<commit_message>
Updates to model policy schedule
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
+++ b/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipK\InputData\plcy-ctrl-ctr\BAEPAbCiPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\ctrl-settings\BAEPAbCiPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821543C2-567D-4203-BA9D-917EA0EB3665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13800"/>
+    <workbookView xWindow="3555" yWindow="435" windowWidth="23595" windowHeight="16230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Source:</t>
   </si>
@@ -36,9 +37,6 @@
     <t>About</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
     <t>This control lever sets whether energy prices are affected by production costs</t>
   </si>
   <si>
@@ -54,9 +52,6 @@
     <t>natural gas</t>
   </si>
   <si>
-    <t>nuclear</t>
-  </si>
-  <si>
     <t>hydro (is not a fuel)</t>
   </si>
   <si>
@@ -99,9 +94,6 @@
     <t>LPG propane or butane</t>
   </si>
   <si>
-    <t>municipal solid waste</t>
-  </si>
-  <si>
     <t>hydrogen</t>
   </si>
   <si>
@@ -111,23 +103,41 @@
     <t>heat</t>
   </si>
   <si>
-    <t>As of EPS 1.5.0, this lever supports the three energy carriers (electricity,</t>
-  </si>
-  <si>
-    <t>district heat, and hydrogen), which tend to be produced and consumed locally.</t>
-  </si>
-  <si>
-    <t>It does not affect other fuel types, whose prices are often determined or influenced</t>
-  </si>
-  <si>
-    <t>by global markets, so domestic producers' costs are less relevant.</t>
+    <t>As of EPS 3.1.0, this lever supports the three energy carriers (electricity,</t>
+  </si>
+  <si>
+    <t>district heat, and hydrogen), as well as fuels produced by the natural gas</t>
+  </si>
+  <si>
+    <t>and petroleum, coal, biomass, and biofuel industries, as noted on the blue tab.</t>
+  </si>
+  <si>
+    <t>municipal solid waste (NOT USED)</t>
+  </si>
+  <si>
+    <t>nuclear (NOT USED)</t>
+  </si>
+  <si>
+    <t>Unit: boolean (1 or 0)</t>
+  </si>
+  <si>
+    <t>In the U.S. model, by default, we allow the suppliers of energy carriers</t>
+  </si>
+  <si>
+    <t>(electricity, district heat, and hydrogen) to pass through changes in their</t>
+  </si>
+  <si>
+    <t>expenses, while other fuel suppliers do not, due to the influence of a global</t>
+  </si>
+  <si>
+    <t>market on setting prices.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +153,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,12 +172,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,14 +188,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,8 +476,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -472,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -490,32 +503,47 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -539,22 +567,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
+      <c r="A1" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -562,23 +590,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -586,7 +614,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -594,7 +622,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -602,7 +630,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -610,7 +638,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -618,7 +646,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -626,7 +654,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -634,7 +662,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -642,23 +670,23 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -666,7 +694,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -674,7 +702,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -682,7 +710,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -690,29 +718,30 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="4">
+      <c r="A22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>